<commit_message>
BD Script With Data Added
</commit_message>
<xml_diff>
--- a/BD.xlsx
+++ b/BD.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MaterialType" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -749,7 +749,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +810,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A2" sqref="A2:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+      <selection activeCell="A2" sqref="A2:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1484,8 +1484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1743,7 +1743,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1812,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+      <selection activeCell="A2" sqref="A2:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2052,7 +2052,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2118,7 +2118,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2187,7 +2187,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2256,7 +2256,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="A2" sqref="A2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>